<commit_message>
Added caliber to model + caliberId parser
</commit_message>
<xml_diff>
--- a/WeaponSystem/WeaponSystem.TestConsoleClient/w.xlsx
+++ b/WeaponSystem/WeaponSystem.TestConsoleClient/w.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="983" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="983" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Pistols" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="106">
   <si>
     <t>Name</t>
   </si>
@@ -169,9 +169,6 @@
     <t>Heckler&amp;Kock</t>
   </si>
   <si>
-    <t>9mm</t>
-  </si>
-  <si>
     <t>http://vignette3.wikia.nocookie.net/cswikia/images/8/81/Mp5hud_cz.png/revision/latest/scale-to-width-down/250?cb=20100730110854</t>
   </si>
   <si>
@@ -190,9 +187,6 @@
     <t>FN Herstal</t>
   </si>
   <si>
-    <t>5.7mm</t>
-  </si>
-  <si>
     <t>http://vignette3.wikia.nocookie.net/cswikia/images/7/78/P90go.png/revision/latest/scale-to-width-down/250?cb=20130813201421</t>
   </si>
   <si>
@@ -226,16 +220,10 @@
     <t>AK-47</t>
   </si>
   <si>
-    <t>7.62mm</t>
-  </si>
-  <si>
     <t>http://vignette4.wikia.nocookie.net/cswikia/images/6/66/Ak47go.png/revision/latest/scale-to-width-down/250?cb=20130813201911</t>
   </si>
   <si>
     <t>AUG</t>
-  </si>
-  <si>
-    <t>5.56mm</t>
   </si>
   <si>
     <t>http://vignette2.wikia.nocookie.net/cswikia/images/e/e9/Auggo.png/revision/latest/scale-to-width-down/250?cb=20130813202013</t>
@@ -476,7 +464,7 @@
   </sheetPr>
   <dimension ref="1:15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -787,7 +775,7 @@
   <dimension ref="1:8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -842,82 +830,82 @@
       <c r="B3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="2" t="n">
+        <v>5.56</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>47</v>
@@ -926,7 +914,7 @@
         <v>0.45</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -949,8 +937,8 @@
   </sheetPr>
   <dimension ref="1:11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -967,7 +955,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -984,142 +972,142 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>67</v>
+        <v>56</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>7.62</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>70</v>
+        <v>59</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>5.56</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>5.56</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>5.56</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>5.56</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>70</v>
+      <c r="C7" s="2" t="n">
+        <v>5.56</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>70</v>
+      <c r="C8" s="2" t="n">
+        <v>5.56</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>70</v>
+      <c r="C9" s="2" t="n">
+        <v>5.56</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>70</v>
+        <v>83</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>5.56</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>70</v>
+        <v>83</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>5.56</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1141,7 +1129,7 @@
   <dimension ref="1:5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1158,7 +1146,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1175,58 +1163,58 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>67</v>
+      <c r="C2" s="2" t="n">
+        <v>7.62</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>67</v>
+        <v>90</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>7.62</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>67</v>
+        <v>93</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>7.62</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>0.5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1248,7 +1236,7 @@
   <dimension ref="1:4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1282,44 +1270,44 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>67</v>
+        <v>99</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>7.62</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>70</v>
+        <v>102</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>5.56</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>5.56</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>